<commit_message>
Update BOU_British_List_tidy.xlsx with revised data entries.
</commit_message>
<xml_diff>
--- a/data/context/BOU_British_List_tidy.xlsx
+++ b/data/context/BOU_British_List_tidy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\agridat-data-services\data-HAU-bbs\data\context\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA08AC3A-AA03-47DA-8380-FC52A3D28CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BB6A89-E70E-4515-85A8-11AFE41C5DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="British_List" sheetId="7" r:id="rId1"/>
@@ -4871,9 +4871,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D641"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12562,7 +12562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D39342BE-1B52-483D-8292-571D6BD8231A}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>